<commit_message>
Added function to calculate energy calcs based on weight and phase
</commit_message>
<xml_diff>
--- a/Data/yatzo alcohol/yatzo_test1/yatzo_test1_TE_DataEntryForm.xlsx
+++ b/Data/yatzo alcohol/yatzo_test1/yatzo_test1_TE_DataEntryForm.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mountain Air\equipment\Ratnoze\DataProcessing\LEMS\LEMS-Data-Processing\Data\yatzo alcohol\yatzo_test1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden\Documents\GitHub\LEMS-Data-Processing\Data\yatzo alcohol\yatzo_test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86986F28-FBCA-47D7-8632-26A53076C532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DF9BEAD-323A-4D1F-A65B-4AF6D8D1D7AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="ThermalEfficiencyInputs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Samuel Bentson</author>
   </authors>
   <commentList>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{7A9DCCA4-64F0-43E8-8EBC-13D5BF460E59}">
+    <comment ref="F35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K35" authorId="0" shapeId="0" xr:uid="{8996DE03-C450-4A44-8D30-6C1CCA31E3CC}">
+    <comment ref="K35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P35" authorId="0" shapeId="0" xr:uid="{7F34AE1B-BF52-47D9-8D31-5DC22F1180CB}">
+    <comment ref="P35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="167">
   <si>
     <t>HIGH POWER TEST (COLD START)</t>
   </si>
@@ -619,20 +618,48 @@
   </si>
   <si>
     <t>alcohol</t>
+  </si>
+  <si>
+    <t>Weighting for voluntary performance Tiers</t>
+  </si>
+  <si>
+    <t>High Power</t>
+  </si>
+  <si>
+    <t>Med Power</t>
+  </si>
+  <si>
+    <t>Low Power</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>weight_total</t>
+  </si>
+  <si>
+    <t>weight_hp</t>
+  </si>
+  <si>
+    <t>weight_mp</t>
+  </si>
+  <si>
+    <t>weight_lp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,6 +715,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -733,7 +771,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1070,12 +1108,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1277,6 +1376,15 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1295,15 +1403,41 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1618,29 +1752,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F031B2B2-166A-4FD0-84C6-B19351E2FA63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.85546875" customWidth="1"/>
-    <col min="22" max="22" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.88671875" customWidth="1"/>
+    <col min="22" max="22" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44"/>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1662,18 +1797,18 @@
       <c r="S1" s="44"/>
       <c r="T1" s="44"/>
     </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44"/>
       <c r="B2" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
       <c r="H2" s="44"/>
       <c r="I2" s="81" t="s">
         <v>137</v>
@@ -1690,18 +1825,18 @@
       <c r="S2" s="44"/>
       <c r="T2" s="44"/>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44"/>
       <c r="B3" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="105">
+      <c r="C3" s="99">
         <v>1</v>
       </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
       <c r="H3" s="44"/>
       <c r="I3" s="84"/>
       <c r="J3" s="60"/>
@@ -1716,18 +1851,18 @@
       <c r="S3" s="44"/>
       <c r="T3" s="44"/>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="44"/>
       <c r="B4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
       <c r="H4" s="44"/>
       <c r="I4" s="84"/>
       <c r="J4" s="60"/>
@@ -1742,18 +1877,18 @@
       <c r="S4" s="44"/>
       <c r="T4" s="44"/>
     </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44"/>
       <c r="B5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
       <c r="H5" s="44"/>
       <c r="I5" s="62"/>
       <c r="J5" s="60"/>
@@ -1768,16 +1903,16 @@
       <c r="S5" s="44"/>
       <c r="T5" s="44"/>
     </row>
-    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="44"/>
       <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
       <c r="H6" s="44"/>
       <c r="I6" s="92" t="s">
         <v>138</v>
@@ -1794,18 +1929,18 @@
       <c r="S6" s="44"/>
       <c r="T6" s="44"/>
     </row>
-    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="105" t="s">
+      <c r="C7" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
       <c r="H7" s="44"/>
       <c r="I7" s="84"/>
       <c r="J7" s="60"/>
@@ -1820,7 +1955,7 @@
       <c r="S7" s="44"/>
       <c r="T7" s="44"/>
     </row>
-    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -1842,7 +1977,7 @@
       <c r="S8" s="44"/>
       <c r="T8" s="44"/>
     </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44"/>
       <c r="B9" s="45"/>
       <c r="C9" s="48" t="s">
@@ -1870,7 +2005,7 @@
       <c r="S9" s="44"/>
       <c r="T9" s="44"/>
     </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44"/>
       <c r="B10" s="15" t="s">
         <v>36</v>
@@ -1900,7 +2035,7 @@
       <c r="S10" s="44"/>
       <c r="T10" s="44"/>
     </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="44"/>
       <c r="B11" s="15" t="s">
         <v>37</v>
@@ -1930,7 +2065,7 @@
       <c r="S11" s="44"/>
       <c r="T11" s="44"/>
     </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="44"/>
       <c r="B12" s="15" t="s">
         <v>117</v>
@@ -1958,7 +2093,7 @@
       <c r="S12" s="44"/>
       <c r="T12" s="44"/>
     </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="44"/>
       <c r="B13" s="15" t="s">
         <v>133</v>
@@ -1986,7 +2121,7 @@
       <c r="S13" s="44"/>
       <c r="T13" s="44"/>
     </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
       <c r="B14" s="15" t="s">
         <v>38</v>
@@ -2016,7 +2151,7 @@
       <c r="S14" s="44"/>
       <c r="T14" s="44"/>
     </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44"/>
       <c r="B15" s="15" t="s">
         <v>118</v>
@@ -2044,7 +2179,7 @@
       <c r="S15" s="44"/>
       <c r="T15" s="44"/>
     </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="44"/>
       <c r="B16" s="20" t="s">
         <v>131</v>
@@ -2076,7 +2211,7 @@
       <c r="S16" s="44"/>
       <c r="T16" s="44"/>
     </row>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="20" t="s">
         <v>28</v>
@@ -2106,7 +2241,7 @@
       <c r="S17" s="44"/>
       <c r="T17" s="44"/>
     </row>
-    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
       <c r="B18" s="20" t="s">
         <v>29</v>
@@ -2134,7 +2269,7 @@
       <c r="S18" s="44"/>
       <c r="T18" s="44"/>
     </row>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="44"/>
       <c r="B19" s="20" t="s">
         <v>30</v>
@@ -2162,7 +2297,7 @@
       <c r="S19" s="44"/>
       <c r="T19" s="44"/>
     </row>
-    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="21" t="s">
         <v>31</v>
@@ -2190,7 +2325,7 @@
       <c r="S20" s="44"/>
       <c r="T20" s="44"/>
     </row>
-    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -2214,20 +2349,20 @@
       <c r="S21" s="44"/>
       <c r="T21" s="44"/>
     </row>
-    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="44"/>
       <c r="B22" s="23" t="s">
         <v>119</v>
       </c>
       <c r="C22" s="52"/>
-      <c r="D22" s="103" t="s">
+      <c r="D22" s="97" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="104"/>
-      <c r="F22" s="103" t="s">
+      <c r="E22" s="98"/>
+      <c r="F22" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="104"/>
+      <c r="G22" s="98"/>
       <c r="H22" s="44"/>
       <c r="I22" s="58"/>
       <c r="J22" s="79"/>
@@ -2242,7 +2377,7 @@
       <c r="S22" s="44"/>
       <c r="T22" s="44"/>
     </row>
-    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="47"/>
       <c r="C23" s="53" t="s">
@@ -2274,7 +2409,7 @@
       <c r="S23" s="44"/>
       <c r="T23" s="44"/>
     </row>
-    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="15" t="s">
         <v>124</v>
@@ -2306,7 +2441,7 @@
       <c r="S24" s="44"/>
       <c r="T24" s="44"/>
     </row>
-    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="44"/>
       <c r="B25" s="15" t="s">
         <v>125</v>
@@ -2338,7 +2473,7 @@
       <c r="S25" s="44"/>
       <c r="T25" s="44"/>
     </row>
-    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="15" t="s">
         <v>126</v>
@@ -2370,7 +2505,7 @@
       <c r="S26" s="44"/>
       <c r="T26" s="44"/>
     </row>
-    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="17" t="s">
         <v>127</v>
@@ -2400,7 +2535,7 @@
       <c r="S27" s="44"/>
       <c r="T27" s="44"/>
     </row>
-    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -2422,7 +2557,7 @@
       <c r="S28" s="44"/>
       <c r="T28" s="44"/>
     </row>
-    <row r="29" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="44"/>
       <c r="B29" s="24"/>
       <c r="C29" s="25"/>
@@ -2450,7 +2585,7 @@
       <c r="S29" s="44"/>
       <c r="T29" s="44"/>
     </row>
-    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="44"/>
       <c r="B30" s="31"/>
       <c r="C30" s="3"/>
@@ -2458,61 +2593,61 @@
         <v>3</v>
       </c>
       <c r="E30" s="16"/>
-      <c r="F30" s="97" t="s">
+      <c r="F30" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="98"/>
+      <c r="G30" s="101"/>
       <c r="H30" s="2"/>
       <c r="I30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J30" s="5"/>
-      <c r="K30" s="97" t="s">
+      <c r="K30" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="L30" s="98"/>
+      <c r="L30" s="101"/>
       <c r="M30" s="2"/>
       <c r="N30" s="16" t="s">
         <v>3</v>
       </c>
       <c r="O30" s="16"/>
-      <c r="P30" s="97" t="s">
+      <c r="P30" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="Q30" s="101"/>
+      <c r="Q30" s="104"/>
       <c r="R30" s="44"/>
       <c r="S30" s="44"/>
       <c r="T30" s="44"/>
     </row>
-    <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="44"/>
       <c r="B31" s="32"/>
       <c r="C31" s="3"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="99" t="s">
+      <c r="F31" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="100"/>
+      <c r="G31" s="103"/>
       <c r="H31" s="2"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="99" t="s">
+      <c r="K31" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="100"/>
+      <c r="L31" s="103"/>
       <c r="M31" s="2"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="99" t="s">
+      <c r="P31" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="Q31" s="102"/>
+      <c r="Q31" s="105"/>
       <c r="R31" s="44"/>
       <c r="S31" s="44"/>
       <c r="T31" s="44"/>
     </row>
-    <row r="32" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="44"/>
       <c r="B32" s="33" t="s">
         <v>6</v>
@@ -2562,7 +2697,7 @@
       <c r="S32" s="44"/>
       <c r="T32" s="44"/>
     </row>
-    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
       <c r="B33" s="34" t="s">
         <v>10</v>
@@ -2612,7 +2747,7 @@
       <c r="S33" s="44"/>
       <c r="T33" s="44"/>
     </row>
-    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="44"/>
       <c r="B34" s="34" t="s">
         <v>12</v>
@@ -2663,7 +2798,7 @@
       <c r="S34" s="44"/>
       <c r="T34" s="44"/>
     </row>
-    <row r="35" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="44"/>
       <c r="B35" s="34" t="s">
         <v>14</v>
@@ -2713,7 +2848,7 @@
       <c r="S35" s="44"/>
       <c r="T35" s="44"/>
     </row>
-    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="44"/>
       <c r="B36" s="37" t="s">
         <v>16</v>
@@ -2751,7 +2886,7 @@
       <c r="S36" s="44"/>
       <c r="T36" s="44"/>
     </row>
-    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="44"/>
       <c r="B37" s="37" t="s">
         <v>17</v>
@@ -2789,7 +2924,7 @@
       <c r="S37" s="44"/>
       <c r="T37" s="44"/>
     </row>
-    <row r="38" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="44"/>
       <c r="B38" s="37" t="s">
         <v>18</v>
@@ -2827,7 +2962,7 @@
       <c r="S38" s="44"/>
       <c r="T38" s="44"/>
     </row>
-    <row r="39" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="44"/>
       <c r="B39" s="34" t="s">
         <v>19</v>
@@ -2877,7 +3012,7 @@
       <c r="S39" s="44"/>
       <c r="T39" s="44"/>
     </row>
-    <row r="40" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="44"/>
       <c r="B40" s="37" t="s">
         <v>20</v>
@@ -2915,7 +3050,7 @@
       <c r="S40" s="44"/>
       <c r="T40" s="44"/>
     </row>
-    <row r="41" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="44"/>
       <c r="B41" s="37" t="s">
         <v>21</v>
@@ -2953,7 +3088,7 @@
       <c r="S41" s="44"/>
       <c r="T41" s="44"/>
     </row>
-    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="44"/>
       <c r="B42" s="37" t="s">
         <v>22</v>
@@ -2991,7 +3126,7 @@
       <c r="S42" s="44"/>
       <c r="T42" s="44"/>
     </row>
-    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44"/>
       <c r="B43" s="34" t="s">
         <v>25</v>
@@ -3029,7 +3164,7 @@
       <c r="S43" s="44"/>
       <c r="T43" s="44"/>
     </row>
-    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="44"/>
       <c r="B44" s="37" t="s">
         <v>23</v>
@@ -3061,7 +3196,7 @@
       <c r="S44" s="44"/>
       <c r="T44" s="44"/>
     </row>
-    <row r="45" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="44"/>
       <c r="B45" s="94" t="s">
         <v>26</v>
@@ -3093,7 +3228,7 @@
       <c r="S45" s="44"/>
       <c r="T45" s="44"/>
     </row>
-    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="44"/>
       <c r="B46" s="44"/>
       <c r="C46" s="44"/>
@@ -3115,12 +3250,14 @@
       <c r="S46" s="44"/>
       <c r="T46" s="44"/>
     </row>
-    <row r="47" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="44"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
+      <c r="B47" s="115" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="116"/>
+      <c r="D47" s="118"/>
+      <c r="E47" s="117"/>
       <c r="F47" s="44"/>
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
@@ -3137,12 +3274,18 @@
       <c r="S47" s="44"/>
       <c r="T47" s="44"/>
     </row>
-    <row r="48" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="44"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
+      <c r="B48" s="113"/>
+      <c r="C48" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="119" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="114" t="s">
+        <v>9</v>
+      </c>
       <c r="F48" s="44"/>
       <c r="G48" s="44"/>
       <c r="H48" s="44"/>
@@ -3159,12 +3302,18 @@
       <c r="S48" s="44"/>
       <c r="T48" s="44"/>
     </row>
-    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="44"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
+      <c r="B49" s="107" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49" s="122"/>
+      <c r="D49" s="108">
+        <v>1</v>
+      </c>
+      <c r="E49" s="110" t="s">
+        <v>164</v>
+      </c>
       <c r="F49" s="44"/>
       <c r="G49" s="44"/>
       <c r="H49" s="44"/>
@@ -3181,12 +3330,18 @@
       <c r="S49" s="44"/>
       <c r="T49" s="44"/>
     </row>
-    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="44"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
+      <c r="B50" s="106" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="122"/>
+      <c r="D50" s="108">
+        <v>1</v>
+      </c>
+      <c r="E50" s="111" t="s">
+        <v>165</v>
+      </c>
       <c r="F50" s="44"/>
       <c r="G50" s="44"/>
       <c r="H50" s="44"/>
@@ -3203,12 +3358,18 @@
       <c r="S50" s="44"/>
       <c r="T50" s="44"/>
     </row>
-    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="44"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="44"/>
+      <c r="B51" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="122"/>
+      <c r="D51" s="108">
+        <v>1</v>
+      </c>
+      <c r="E51" s="111" t="s">
+        <v>166</v>
+      </c>
       <c r="F51" s="44"/>
       <c r="G51" s="44"/>
       <c r="H51" s="44"/>
@@ -3225,12 +3386,19 @@
       <c r="S51" s="44"/>
       <c r="T51" s="44"/>
     </row>
-    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="44"/>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
+      <c r="B52" s="109" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52" s="123"/>
+      <c r="D52" s="120">
+        <f>SUM(D49:D51)</f>
+        <v>3</v>
+      </c>
+      <c r="E52" s="112" t="s">
+        <v>163</v>
+      </c>
       <c r="F52" s="44"/>
       <c r="G52" s="44"/>
       <c r="H52" s="44"/>
@@ -3247,7 +3415,7 @@
       <c r="S52" s="44"/>
       <c r="T52" s="44"/>
     </row>
-    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="44"/>
       <c r="B53" s="44"/>
       <c r="C53" s="44"/>
@@ -3269,7 +3437,7 @@
       <c r="S53" s="44"/>
       <c r="T53" s="44"/>
     </row>
-    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="44"/>
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
@@ -3291,7 +3459,7 @@
       <c r="S54" s="44"/>
       <c r="T54" s="44"/>
     </row>
-    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="44"/>
       <c r="B55" s="44"/>
       <c r="C55" s="44"/>
@@ -3313,7 +3481,7 @@
       <c r="S55" s="44"/>
       <c r="T55" s="44"/>
     </row>
-    <row r="56" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="44"/>
       <c r="B56" s="44"/>
       <c r="C56" s="44"/>
@@ -3335,7 +3503,7 @@
       <c r="S56" s="44"/>
       <c r="T56" s="44"/>
     </row>
-    <row r="57" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="44"/>
       <c r="B57" s="44"/>
       <c r="C57" s="44"/>
@@ -3357,7 +3525,7 @@
       <c r="S57" s="44"/>
       <c r="T57" s="44"/>
     </row>
-    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="44"/>
       <c r="B58" s="44"/>
       <c r="C58" s="44"/>
@@ -3379,7 +3547,7 @@
       <c r="S58" s="44"/>
       <c r="T58" s="44"/>
     </row>
-    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="44"/>
       <c r="B59" s="44"/>
       <c r="C59" s="44"/>
@@ -3401,7 +3569,7 @@
       <c r="S59" s="44"/>
       <c r="T59" s="44"/>
     </row>
-    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="44"/>
       <c r="B60" s="44"/>
       <c r="C60" s="44"/>
@@ -3423,7 +3591,7 @@
       <c r="S60" s="44"/>
       <c r="T60" s="44"/>
     </row>
-    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="44"/>
       <c r="B61" s="44"/>
       <c r="C61" s="44"/>
@@ -3445,7 +3613,7 @@
       <c r="S61" s="44"/>
       <c r="T61" s="44"/>
     </row>
-    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="44"/>
       <c r="B62" s="44"/>
       <c r="C62" s="44"/>
@@ -3467,7 +3635,7 @@
       <c r="S62" s="44"/>
       <c r="T62" s="44"/>
     </row>
-    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="44"/>
       <c r="B63" s="44"/>
       <c r="C63" s="44"/>
@@ -3489,7 +3657,7 @@
       <c r="S63" s="44"/>
       <c r="T63" s="44"/>
     </row>
-    <row r="64" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="44"/>
       <c r="B64" s="44"/>
       <c r="C64" s="44"/>
@@ -3511,7 +3679,7 @@
       <c r="S64" s="44"/>
       <c r="T64" s="44"/>
     </row>
-    <row r="65" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="44"/>
       <c r="B65" s="44"/>
       <c r="C65" s="44"/>
@@ -3533,7 +3701,7 @@
       <c r="S65" s="44"/>
       <c r="T65" s="44"/>
     </row>
-    <row r="66" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="44"/>
       <c r="B66" s="44"/>
       <c r="C66" s="44"/>
@@ -3555,7 +3723,7 @@
       <c r="S66" s="44"/>
       <c r="T66" s="44"/>
     </row>
-    <row r="67" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="44"/>
       <c r="B67" s="44"/>
       <c r="C67" s="44"/>
@@ -3577,7 +3745,7 @@
       <c r="S67" s="44"/>
       <c r="T67" s="44"/>
     </row>
-    <row r="68" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="44"/>
       <c r="B68" s="44"/>
       <c r="C68" s="44"/>
@@ -3599,7 +3767,7 @@
       <c r="S68" s="44"/>
       <c r="T68" s="44"/>
     </row>
-    <row r="69" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="44"/>
       <c r="B69" s="44"/>
       <c r="C69" s="44"/>
@@ -3621,7 +3789,7 @@
       <c r="S69" s="44"/>
       <c r="T69" s="44"/>
     </row>
-    <row r="70" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="44"/>
       <c r="B70" s="44"/>
       <c r="C70" s="44"/>
@@ -3643,7 +3811,7 @@
       <c r="S70" s="44"/>
       <c r="T70" s="44"/>
     </row>
-    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="44"/>
       <c r="B71" s="44"/>
       <c r="C71" s="44"/>
@@ -3665,7 +3833,7 @@
       <c r="S71" s="44"/>
       <c r="T71" s="44"/>
     </row>
-    <row r="72" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="44"/>
       <c r="B72" s="44"/>
       <c r="C72" s="44"/>
@@ -3687,7 +3855,7 @@
       <c r="S72" s="44"/>
       <c r="T72" s="44"/>
     </row>
-    <row r="73" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="44"/>
       <c r="B73" s="44"/>
       <c r="C73" s="44"/>
@@ -3709,7 +3877,7 @@
       <c r="S73" s="44"/>
       <c r="T73" s="44"/>
     </row>
-    <row r="74" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="44"/>
       <c r="B74" s="44"/>
       <c r="C74" s="44"/>
@@ -3731,7 +3899,7 @@
       <c r="S74" s="44"/>
       <c r="T74" s="44"/>
     </row>
-    <row r="75" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="44"/>
       <c r="B75" s="44"/>
       <c r="C75" s="44"/>
@@ -3753,7 +3921,7 @@
       <c r="S75" s="44"/>
       <c r="T75" s="44"/>
     </row>
-    <row r="76" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="44"/>
       <c r="B76" s="44"/>
       <c r="C76" s="44"/>
@@ -3775,7 +3943,7 @@
       <c r="S76" s="44"/>
       <c r="T76" s="44"/>
     </row>
-    <row r="77" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="44"/>
       <c r="B77" s="44"/>
       <c r="C77" s="44"/>
@@ -3797,7 +3965,7 @@
       <c r="S77" s="44"/>
       <c r="T77" s="44"/>
     </row>
-    <row r="78" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="44"/>
       <c r="B78" s="44"/>
       <c r="C78" s="44"/>
@@ -3819,7 +3987,7 @@
       <c r="S78" s="44"/>
       <c r="T78" s="44"/>
     </row>
-    <row r="79" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="44"/>
       <c r="B79" s="44"/>
       <c r="C79" s="44"/>
@@ -3841,7 +4009,7 @@
       <c r="S79" s="44"/>
       <c r="T79" s="44"/>
     </row>
-    <row r="80" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="44"/>
       <c r="B80" s="44"/>
       <c r="C80" s="44"/>
@@ -3863,7 +4031,7 @@
       <c r="S80" s="44"/>
       <c r="T80" s="44"/>
     </row>
-    <row r="81" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="44"/>
       <c r="B81" s="44"/>
       <c r="C81" s="44"/>
@@ -3885,7 +4053,7 @@
       <c r="S81" s="44"/>
       <c r="T81" s="44"/>
     </row>
-    <row r="82" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="44"/>
       <c r="B82" s="44"/>
       <c r="C82" s="44"/>
@@ -3907,7 +4075,7 @@
       <c r="S82" s="44"/>
       <c r="T82" s="44"/>
     </row>
-    <row r="83" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="44"/>
       <c r="B83" s="44"/>
       <c r="C83" s="44"/>
@@ -3929,7 +4097,7 @@
       <c r="S83" s="44"/>
       <c r="T83" s="44"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="44"/>
       <c r="B84" s="44"/>
       <c r="C84" s="44"/>
@@ -3951,11 +4119,8 @@
       <c r="S84" s="44"/>
       <c r="T84" s="44"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="44"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="44"/>
-      <c r="D85" s="44"/>
       <c r="E85" s="44"/>
       <c r="F85" s="44"/>
       <c r="G85" s="44"/>
@@ -3973,11 +4138,8 @@
       <c r="S85" s="44"/>
       <c r="T85" s="44"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="44"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44"/>
       <c r="E86" s="44"/>
       <c r="F86" s="44"/>
       <c r="G86" s="44"/>
@@ -3997,6 +4159,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="P31:Q31"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="C2:G2"/>
@@ -4005,12 +4173,6 @@
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="P31:Q31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>